<commit_message>
Prep Topics 1 and 2
</commit_message>
<xml_diff>
--- a/topic01-introduction/unit-01a-lectures/talk-2/calendars.xlsx
+++ b/topic01-introduction/unit-01a-lectures/talk-2/calendars.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maireadmeagher/Documents/GitRepos/fp-24/topic01-introduction/unit-01a-lectures/talk-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CA7E76-4DBF-5248-A75F-1A8BB90634EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B6DD73-AD57-434F-A6B6-1F80B10CCE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4760" yWindow="1080" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1880" yWindow="1880" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,9 +71,6 @@
     <t>APR</t>
   </si>
   <si>
-    <t>SEMESTER 1</t>
-  </si>
-  <si>
     <t>MAY</t>
   </si>
   <si>
@@ -108,6 +105,9 @@
   </si>
   <si>
     <t>Weight</t>
+  </si>
+  <si>
+    <t>SEMESTER 8</t>
   </si>
 </sst>
 </file>
@@ -131,7 +131,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,6 +162,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -249,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -271,24 +277,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -315,6 +321,18 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -692,9 +710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -711,23 +727,23 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="7" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -745,13 +761,13 @@
         <v>3</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="24" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -761,15 +777,15 @@
       <c r="C3" s="4">
         <v>15</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <f>+C3+1</f>
         <v>16</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="26">
         <f>+D3+1</f>
         <v>17</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="4">
         <f>+E3+1</f>
         <v>18</v>
       </c>
@@ -777,7 +793,7 @@
         <f>+F3+1</f>
         <v>19</v>
       </c>
-      <c r="L3" s="11"/>
+      <c r="L3" s="13"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
@@ -787,19 +803,19 @@
         <f t="shared" ref="C4" si="0">C3+7</f>
         <v>22</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <v>26</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="26">
         <v>27</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="4">
         <v>28</v>
       </c>
       <c r="G4" s="2">
         <v>28</v>
       </c>
-      <c r="L4" s="11"/>
+      <c r="L4" s="13"/>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -813,14 +829,14 @@
         <f>C4+7</f>
         <v>29</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
         <v>1</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="26">
         <f t="shared" ref="E5:G5" si="1">+D5+1</f>
         <v>2</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="4">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -841,15 +857,15 @@
       <c r="C6" s="4">
         <v>5</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4">
         <f>C6+1</f>
         <v>6</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="26">
         <f t="shared" ref="E6:F6" si="2">D6+1</f>
         <v>7</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="25">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
@@ -857,8 +873,8 @@
         <f t="shared" ref="G6" si="3">F6+1</f>
         <v>9</v>
       </c>
-      <c r="L6" s="13" t="s">
-        <v>18</v>
+      <c r="L6" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="M6" s="16">
         <v>0.05</v>
@@ -870,20 +886,20 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
-      <c r="L7" s="11"/>
+      <c r="L7" s="13"/>
       <c r="M7" s="3"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -894,15 +910,15 @@
         <f>C6+14</f>
         <v>19</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="4">
         <f>D6+14</f>
         <v>20</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="26">
         <f>E6+14</f>
         <v>21</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="4">
         <f>F6+7</f>
         <v>15</v>
       </c>
@@ -910,7 +926,7 @@
         <f>G6+7</f>
         <v>16</v>
       </c>
-      <c r="L8" s="11"/>
+      <c r="L8" s="13"/>
       <c r="M8" s="2"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -924,15 +940,15 @@
         <f>C8+7</f>
         <v>26</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="4">
         <f t="shared" ref="D9:E9" si="4">D8+7</f>
         <v>27</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="26">
         <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="4">
         <v>29</v>
       </c>
       <c r="G9" s="2">
@@ -951,15 +967,15 @@
       <c r="C10" s="4">
         <v>4</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="4">
         <f t="shared" ref="D10:G19" si="5">C10+1</f>
         <v>5</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="26">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="25">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
@@ -968,7 +984,7 @@
         <v>8</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M10" s="16">
         <v>0.05</v>
@@ -982,15 +998,15 @@
         <f>C10+7</f>
         <v>11</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="4">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="26">
         <f t="shared" si="5"/>
         <v>13</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="4">
         <f t="shared" si="5"/>
         <v>14</v>
       </c>
@@ -999,7 +1015,7 @@
         <v>15</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="M11" s="20">
         <v>0.4</v>
@@ -1013,15 +1029,15 @@
         <f t="shared" ref="C12" si="6">C11+7</f>
         <v>18</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="4">
         <f t="shared" si="5"/>
         <v>19</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="26">
         <f t="shared" si="5"/>
         <v>20</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="4">
         <f t="shared" si="5"/>
         <v>21</v>
       </c>
@@ -1030,9 +1046,9 @@
         <v>22</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="L12" s="9"/>
+        <v>19</v>
+      </c>
+      <c r="L12" s="10"/>
       <c r="M12" s="21"/>
     </row>
     <row r="13" spans="1:13" s="1" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -1067,7 +1083,7 @@
       </c>
       <c r="J13"/>
       <c r="K13"/>
-      <c r="L13" s="9"/>
+      <c r="L13" s="10"/>
       <c r="M13" s="21"/>
     </row>
     <row r="14" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1095,7 +1111,7 @@
       </c>
       <c r="J14"/>
       <c r="K14"/>
-      <c r="L14" s="9"/>
+      <c r="L14" s="10"/>
       <c r="M14" s="21"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -1106,23 +1122,23 @@
         <f>C14+7</f>
         <v>8</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="4">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="26">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="4">
         <f t="shared" si="5"/>
         <v>11</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="26">
         <f t="shared" si="5"/>
         <v>12</v>
       </c>
-      <c r="L15" s="9"/>
+      <c r="L15" s="10"/>
       <c r="M15" s="21"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1133,15 +1149,15 @@
         <f t="shared" ref="C16:F16" si="8">C15+7</f>
         <v>15</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="4">
         <f t="shared" si="5"/>
         <v>16</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="26">
         <f t="shared" si="8"/>
         <v>17</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="4">
         <f t="shared" si="8"/>
         <v>18</v>
       </c>
@@ -1149,7 +1165,7 @@
         <f t="shared" ref="G16" si="9">G15+7</f>
         <v>19</v>
       </c>
-      <c r="L16" s="9"/>
+      <c r="L16" s="11"/>
       <c r="M16" s="22"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
@@ -1160,14 +1176,14 @@
         <f t="shared" ref="C17" si="10">C16+7</f>
         <v>22</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="4">
         <f t="shared" si="5"/>
         <v>23</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="26">
         <v>1</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="4">
         <v>2</v>
       </c>
       <c r="G17" s="2">
@@ -1198,12 +1214,12 @@
       </c>
       <c r="J18"/>
       <c r="K18"/>
-      <c r="L18" s="10"/>
+      <c r="L18" s="12"/>
       <c r="M18" s="2"/>
     </row>
     <row r="19" spans="1:13" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>5</v>
@@ -1224,12 +1240,12 @@
         <v>8</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J19"/>
       <c r="K19"/>
-      <c r="L19" s="12" t="s">
-        <v>22</v>
+      <c r="L19" s="27" t="s">
+        <v>21</v>
       </c>
       <c r="M19" s="23">
         <v>0.5</v>
@@ -1237,7 +1253,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>